<commit_message>
cập nhật kế hoạch phân công tuần 5 (26/10/22)
cập nhật kế hoạch phân công tuần 5 (26/10/22)
</commit_message>
<xml_diff>
--- a/plan/kehoachphancong_tuan5.xlsx
+++ b/plan/kehoachphancong_tuan5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comeh\Documents\GitHub\Do_An_Quan_Ly_Phong_Game\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26193EE-BB9C-4AA6-B51F-E6D761935D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEDEE26-6275-4E62-B06B-75474BF6E9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
   <si>
     <t>KẾ HOẠCH PHÂN CÔNG HÀNG TUẦN</t>
   </si>
@@ -142,12 +142,6 @@
   <si>
     <t>[maytinh.hpp]
 Viết hàm:
-- Đọc danh sách máy tính từ thư mục "../File/danhsachmaytinh.txt"
-- Xóa một máy tính từ danh sách</t>
-  </si>
-  <si>
-    <t>[maytinh.hpp]
-Viết hàm:
 - Chỉnh sửa thông tin của một máy tính trong danh sách bằng mã máy tính. Chỉ được thay đổi thông tin số máy và kiểu máy</t>
   </si>
   <si>
@@ -165,6 +159,51 @@
 + 3. Xóa máy tính
 + 4. Chỉnh sửa thông tin máy tính
 - Gọi menu vào file main.cpp</t>
+  </si>
+  <si>
+    <t>[xuly.hpp]
+Viết hàm:
+- Chuẩn hóa tên tài khoản thành in thường toàn bộ các kí tự, không có khoảng trắng thừa</t>
+  </si>
+  <si>
+    <t>[khachhang.hpp]
+Viết hàm:
+- Chuyển cây sang mảng
+- Sắp xếp danh sách khách hàng theo mã khách hàng</t>
+  </si>
+  <si>
+    <t>[khachhang.hpp]
+Viết hàm:
+- In danh sách khách hàng theo chiều dọc/ngang
+- Giải phóng danh sách khách hàng</t>
+  </si>
+  <si>
+    <t>[khachhang.hpp]
+Viết hàm:
+- Xóa khách hàng ra khỏi danh sách</t>
+  </si>
+  <si>
+    <t>[khachhang.hpp]
+Viết hàm:
+- Nhập và thêm một khách hàng vào danh sách
+- Tạo mã khách hàng (một số ngẫu nhiên từ 100 đến 999)
+- Kiểm tra mã khách hàng đã tồn tại hay chưa</t>
+  </si>
+  <si>
+    <t>[khachhang.hpp]
+Viết hàm:
+- Chỉnh sửa thông tin của một khách hàng trong danh sách khách hàng bằng số điện thoại. Chỉ được thay đổi thông tin tài khoản và mật khẩu</t>
+  </si>
+  <si>
+    <t>[khachhang.hpp]
+Viết hàm:
+- Đọc danh sách khách hàng từ file "../File/danhsachkhachhang.txt"</t>
+  </si>
+  <si>
+    <t>[maytinh.hpp]
+Viết hàm:
+- Đọc danh sách máy tính từ file "../File/danhsachmaytinh.txt"
+- Xóa một máy tính từ danh sách</t>
   </si>
 </sst>
 </file>
@@ -426,6 +465,18 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -439,18 +490,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2069,7 +2108,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2080,204 +2119,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
     </row>
     <row r="9" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15" t="s">
+      <c r="C9" s="18"/>
+      <c r="D9" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="16" t="s">
+      <c r="E9" s="18"/>
+      <c r="F9" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="16"/>
-      <c r="H9" s="15" t="s">
+      <c r="G9" s="20"/>
+      <c r="H9" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="14"/>
-      <c r="J9" s="16" t="s">
+      <c r="I9" s="18"/>
+      <c r="J9" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="16"/>
-      <c r="L9" s="15" t="s">
+      <c r="K9" s="20"/>
+      <c r="L9" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="14"/>
-      <c r="N9" s="15" t="s">
+      <c r="M9" s="18"/>
+      <c r="N9" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="O9" s="16"/>
+      <c r="O9" s="20"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="17" t="s">
+      <c r="C10" s="15"/>
+      <c r="D10" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="18" t="s">
+      <c r="E10" s="15"/>
+      <c r="F10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="18"/>
-      <c r="H10" s="17" t="s">
+      <c r="G10" s="13"/>
+      <c r="H10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I10" s="20"/>
-      <c r="J10" s="18" t="s">
+      <c r="I10" s="15"/>
+      <c r="J10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="18"/>
-      <c r="L10" s="17" t="s">
+      <c r="K10" s="13"/>
+      <c r="L10" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="M10" s="20"/>
-      <c r="N10" s="17" t="s">
+      <c r="M10" s="15"/>
+      <c r="N10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="O10" s="18"/>
+      <c r="O10" s="13"/>
     </row>
     <row r="11" spans="1:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
@@ -2397,7 +2436,7 @@
     </row>
     <row r="15" spans="1:15" ht="91.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
@@ -2420,7 +2459,7 @@
     </row>
     <row r="16" spans="1:15" ht="94.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
@@ -2443,7 +2482,7 @@
     </row>
     <row r="17" spans="1:15" ht="98.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
@@ -2466,7 +2505,7 @@
     </row>
     <row r="18" spans="1:15" ht="154.80000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
@@ -2487,11 +2526,15 @@
       <c r="N18" s="7"/>
       <c r="O18" s="8"/>
     </row>
-    <row r="19" spans="1:15" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
+    <row r="19" spans="1:15" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
+      <c r="D19" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="E19" s="10"/>
       <c r="F19" s="7"/>
       <c r="G19" s="8"/>
@@ -2505,10 +2548,14 @@
       <c r="O19" s="8"/>
     </row>
     <row r="20" spans="1:15" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
+      <c r="A20" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
+      <c r="D20" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="E20" s="10"/>
       <c r="F20" s="7"/>
       <c r="G20" s="8"/>
@@ -2521,11 +2568,15 @@
       <c r="N20" s="7"/>
       <c r="O20" s="8"/>
     </row>
-    <row r="21" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
+    <row r="21" spans="1:15" ht="83.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
-      <c r="D21" s="9"/>
+      <c r="D21" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="E21" s="10"/>
       <c r="F21" s="7"/>
       <c r="G21" s="8"/>
@@ -2538,11 +2589,15 @@
       <c r="N21" s="7"/>
       <c r="O21" s="8"/>
     </row>
-    <row r="22" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
+    <row r="22" spans="1:15" ht="79.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>31</v>
+      </c>
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
-      <c r="D22" s="9"/>
+      <c r="D22" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="E22" s="10"/>
       <c r="F22" s="7"/>
       <c r="G22" s="8"/>
@@ -2555,11 +2610,15 @@
       <c r="N22" s="7"/>
       <c r="O22" s="8"/>
     </row>
-    <row r="23" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
+    <row r="23" spans="1:15" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
+      <c r="D23" s="9" t="s">
+        <v>4</v>
+      </c>
       <c r="E23" s="10"/>
       <c r="F23" s="7"/>
       <c r="G23" s="8"/>
@@ -2572,11 +2631,15 @@
       <c r="N23" s="7"/>
       <c r="O23" s="8"/>
     </row>
-    <row r="24" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
+    <row r="24" spans="1:15" ht="103.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
-      <c r="D24" s="9"/>
+      <c r="D24" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="E24" s="10"/>
       <c r="F24" s="7"/>
       <c r="G24" s="8"/>
@@ -2589,11 +2652,15 @@
       <c r="N24" s="7"/>
       <c r="O24" s="8"/>
     </row>
-    <row r="25" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
+    <row r="25" spans="1:15" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
-      <c r="D25" s="9"/>
+      <c r="D25" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="E25" s="10"/>
       <c r="F25" s="7"/>
       <c r="G25" s="8"/>
@@ -2659,13 +2726,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
     <mergeCell ref="A1:O8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
@@ -2674,6 +2734,13 @@
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="N9:O9"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập ngày đầu tiên trong tuần đối với lịch biểu việc nhà." sqref="B10" xr:uid="{00000000-0002-0000-0000-000000000000}"/>

</xml_diff>